<commit_message>
fix parameterization, run strategy and influence experiments
</commit_message>
<xml_diff>
--- a/parameter_files/base/de_dg_gwq_lower.xlsx
+++ b/parameter_files/base/de_dg_gwq_lower.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4efc3e9dc81381f4/Documents/SJV-gen-modeling/parameter_files/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{497C6D93-B399-4E40-8368-389B57572BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DA97E34-0BA3-4DF7-8D81-7CC4CB0EBE32}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{497C6D93-B399-4E40-8368-389B57572BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17285F42-A4DA-44AF-BDC1-83BF948B976D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{761CEF3E-82D4-4F85-B34A-FACCDF66C57E}"/>
+    <workbookView xWindow="1100" yWindow="1190" windowWidth="14400" windowHeight="7360" xr2:uid="{761CEF3E-82D4-4F85-B34A-FACCDF66C57E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -650,10 +650,10 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M3" sqref="M3"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -983,10 +983,18 @@
         <v>10</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="C24" s="6">
+        <v>-0.5</v>
+      </c>
+      <c r="D24" s="6">
+        <v>-0.5</v>
+      </c>
+      <c r="E24" s="6">
+        <v>-0.5</v>
+      </c>
+      <c r="F24" s="6">
+        <v>-0.5</v>
+      </c>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -994,16 +1002,16 @@
         <v>11</v>
       </c>
       <c r="B25" s="4"/>
-      <c r="C25" s="6">
-        <v>-0.5</v>
-      </c>
-      <c r="D25" s="6">
-        <v>-0.5</v>
-      </c>
-      <c r="E25" s="6">
-        <v>-0.5</v>
-      </c>
-      <c r="F25" s="6">
+      <c r="C25" s="4">
+        <v>-0.5</v>
+      </c>
+      <c r="D25" s="4">
+        <v>-0.5</v>
+      </c>
+      <c r="E25" s="4">
+        <v>-0.5</v>
+      </c>
+      <c r="F25" s="4">
         <v>-0.5</v>
       </c>
       <c r="G25" s="4"/>
@@ -1013,18 +1021,6 @@
         <v>12</v>
       </c>
       <c r="B26" s="4"/>
-      <c r="C26" s="4">
-        <v>-0.5</v>
-      </c>
-      <c r="D26" s="4">
-        <v>-0.5</v>
-      </c>
-      <c r="E26" s="4">
-        <v>-0.5</v>
-      </c>
-      <c r="F26" s="4">
-        <v>-0.5</v>
-      </c>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
add parameter comparison code, change base and v4 parameterizations
</commit_message>
<xml_diff>
--- a/parameter_files/base/de_dg_gwq_lower.xlsx
+++ b/parameter_files/base/de_dg_gwq_lower.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4efc3e9dc81381f4/Documents/SJV-gen-modeling/parameter_files/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{497C6D93-B399-4E40-8368-389B57572BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17285F42-A4DA-44AF-BDC1-83BF948B976D}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{497C6D93-B399-4E40-8368-389B57572BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55112D42-B422-43C5-AB83-87F939262E1E}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1190" windowWidth="14400" windowHeight="7360" xr2:uid="{761CEF3E-82D4-4F85-B34A-FACCDF66C57E}"/>
+    <workbookView xWindow="20" yWindow="520" windowWidth="19180" windowHeight="10060" xr2:uid="{761CEF3E-82D4-4F85-B34A-FACCDF66C57E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -639,7 +639,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -650,18 +650,18 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6328125" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>27</v>
@@ -685,7 +685,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
@@ -696,7 +696,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
@@ -707,7 +707,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>16</v>
       </c>
@@ -718,7 +718,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>17</v>
       </c>
@@ -729,7 +729,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>18</v>
       </c>
@@ -740,7 +740,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>19</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>20</v>
       </c>
@@ -772,7 +772,7 @@
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>21</v>
       </c>
@@ -791,7 +791,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
@@ -802,7 +802,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
@@ -813,7 +813,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -824,7 +824,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
@@ -835,7 +835,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
@@ -846,7 +846,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>23</v>
       </c>
@@ -857,7 +857,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>24</v>
       </c>
@@ -868,7 +868,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>25</v>
       </c>
@@ -881,26 +881,18 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="5"/>
-      <c r="C18" s="10">
-        <v>-0.5</v>
-      </c>
-      <c r="D18" s="10">
-        <v>-0.5</v>
-      </c>
-      <c r="E18" s="10">
-        <v>-0.5</v>
-      </c>
-      <c r="F18" s="10">
-        <v>-0.5</v>
-      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
@@ -919,7 +911,7 @@
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
@@ -930,7 +922,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -943,7 +935,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>8</v>
       </c>
@@ -967,7 +959,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -978,7 +970,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>10</v>
       </c>
@@ -997,7 +989,7 @@
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>11</v>
       </c>
@@ -1016,14 +1008,14 @@
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>13</v>
       </c>

</xml_diff>